<commit_message>
Add coroutine system and improve animation FSM tools
Introduced a new CoroutineSystem with manager, example, and editor debugger for handling coroutines with owner/tag support. Enhanced the animation FSM generator and related scripts: added state path support, transition/condition serialization, and generated hash classes for animator states. Refactored WarriorController and related FSM state classes for improved modularity and maintainability. Updated BackpackTable and LocalizationTable assets, and made minor improvements to other systems.
</commit_message>
<xml_diff>
--- a/Assets/YusGameFrame/ExcelTool/Excels/Localization.xlsx
+++ b/Assets/YusGameFrame/ExcelTool/Excels/Localization.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>key</t>
   </si>
@@ -57,6 +57,15 @@
   </si>
   <si>
     <t>person</t>
+  </si>
+  <si>
+    <t>t1</t>
+  </si>
+  <si>
+    <t>&lt;link="glitch"&gt;是故障！~!&lt;/link&gt;</t>
+  </si>
+  <si>
+    <t>&lt;link="wave"&gt;wave, wave, wave, alright&lt;/link&gt;</t>
   </si>
 </sst>
 </file>
@@ -987,16 +996,17 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="4" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="5" outlineLevelCol="2"/>
   <cols>
     <col min="2" max="2" width="49.8181818181818" customWidth="1"/>
     <col min="3" max="3" width="50.0909090909091" customWidth="1"/>
+    <col min="4" max="4" width="34.8181818181818" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1046,6 +1056,17 @@
       </c>
       <c r="C5" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>